<commit_message>
Reading data from Excel through Hashmap
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -5,17 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sayan Ghosh Dastidar\RestAssuredLearning\ExcelReading\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sayan Ghosh Dastidar\RestAssuredLearning\RestAssuredFrameworkExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927FD32C-5E22-46F5-8B81-57B335A7C251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F1CC59-616F-4E0A-8810-2C34CC798781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sample" sheetId="3" r:id="rId2"/>
-    <sheet name="Demo" sheetId="2" r:id="rId3"/>
+    <sheet name="Library API" sheetId="5" r:id="rId1"/>
+    <sheet name="TestData" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Data1</t>
   </si>
@@ -87,6 +86,39 @@
   </si>
   <si>
     <t>22www</t>
+  </si>
+  <si>
+    <t>Library - Add Book</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>4141</t>
+  </si>
+  <si>
+    <t>Sayan GD</t>
+  </si>
+  <si>
+    <t>Appium with Java</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>Aisle</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Add Book</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
   </si>
 </sst>
 </file>
@@ -149,10 +181,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,114 +465,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E981BB76-3CD9-433C-AD28-D03BE3681EDA}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8948485C-9701-4375-A537-500D0D9C6713}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3920982-C4EB-462A-A9B0-25AB034BC8F5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Delete Book method
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sayan Ghosh Dastidar\RestAssuredLearning\RestAssuredFrameworkExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F1CC59-616F-4E0A-8810-2C34CC798781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9A499B-0FE4-4FE1-AE37-80B2CC213A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
     <t>Add Book</t>
   </si>
   <si>
-    <t>ABCDEF</t>
+    <t>XYZ</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>